<commit_message>
Filling out the installation codes
</commit_message>
<xml_diff>
--- a/docs/Devices.xlsx
+++ b/docs/Devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AllanK\Desktop\Courses\IV Semester\Statistics\Silicon Showdown\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C664375C-9061-4641-A356-41A2E56A305B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB53300-D577-4AEE-9144-93B68804A822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7120F2FA-3539-4123-B25C-F19AAF0F0EE0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Allan</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>M1</t>
+  </si>
+  <si>
+    <t>Walid</t>
+  </si>
+  <si>
+    <t>RTX 4070</t>
   </si>
 </sst>
 </file>
@@ -512,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E337D42-F98A-4DDD-80BA-EA16F428AD29}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,6 +671,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>